<commit_message>
Updated CV plots with separate y-axes
</commit_message>
<xml_diff>
--- a/examples/Test_Knot_Number/output_bias.correct_FALSE/GOA POP Indices.xlsx
+++ b/examples/Test_Knot_Number/output_bias.correct_FALSE/GOA POP Indices.xlsx
@@ -1,20 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nmfs.local\AKC-ABL\Users\curry.cunningham\My Documents\Projects\VAST Evaluation\AFSC_VAST_Evaluation\examples\Test_Knot_Number\output_bias.correct_FALSE\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <workbookPr date1904="false"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15135" windowHeight="9090"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="plot.list" sheetId="1" r:id="rId1"/>
+    <sheet name="plot.list" r:id="rId3" sheetId="1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -423,39 +416,23 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
+      <patternFill patternType="darkGray"/>
     </fill>
   </fills>
   <borders count="1">
@@ -467,309 +444,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Comma" xfId="1" builtinId="3"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-  </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="44546A"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="5B9BD5"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="ED7D31"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="FFC000"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4472C4"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="70AD47"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0563C1"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="954F72"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
-                <a:tint val="94000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst/>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
-</a:theme>
-</file>
-
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J113"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:K113"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1">
+      <c r="A1"/>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -798,20 +491,20 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
-        <v>1984</v>
-      </c>
-      <c r="C2">
-        <v>558907.52161941363</v>
-      </c>
-      <c r="D2">
-        <v>91234.248287679467</v>
-      </c>
-      <c r="E2">
+      <c r="B2" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C2" t="n">
+        <v>558907.5216194136</v>
+      </c>
+      <c r="D2" t="n">
+        <v>91234.24828767947</v>
+      </c>
+      <c r="E2" t="n">
         <v>0.1632367516245472</v>
       </c>
       <c r="F2" t="s">
@@ -830,20 +523,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3">
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
-        <v>1987</v>
-      </c>
-      <c r="C3">
-        <v>461946.41793006018</v>
-      </c>
-      <c r="D3">
-        <v>88031.866432872004</v>
-      </c>
-      <c r="E3">
+      <c r="B3" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C3" t="n">
+        <v>461946.4179300602</v>
+      </c>
+      <c r="D3" t="n">
+        <v>88031.866432872</v>
+      </c>
+      <c r="E3" t="n">
         <v>0.19056726714612224</v>
       </c>
       <c r="F3" t="s">
@@ -862,20 +555,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4">
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
-        <v>1990</v>
-      </c>
-      <c r="C4">
-        <v>547370.93565172621</v>
-      </c>
-      <c r="D4">
-        <v>94994.290302851761</v>
-      </c>
-      <c r="E4">
+      <c r="B4" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C4" t="n">
+        <v>547370.9356517262</v>
+      </c>
+      <c r="D4" t="n">
+        <v>94994.29030285176</v>
+      </c>
+      <c r="E4" t="n">
         <v>0.17354646386137945</v>
       </c>
       <c r="F4" t="s">
@@ -894,20 +587,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
-        <v>1993</v>
-      </c>
-      <c r="C5">
-        <v>785314.30946206558</v>
-      </c>
-      <c r="D5">
-        <v>136766.43960182829</v>
-      </c>
-      <c r="E5">
+      <c r="B5" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C5" t="n">
+        <v>785314.3094620656</v>
+      </c>
+      <c r="D5" t="n">
+        <v>136766.4396018283</v>
+      </c>
+      <c r="E5" t="n">
         <v>0.17415503315546646</v>
       </c>
       <c r="F5" t="s">
@@ -926,20 +619,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6">
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
-        <v>1996</v>
-      </c>
-      <c r="C6">
-        <v>984018.70994085993</v>
-      </c>
-      <c r="D6">
+      <c r="B6" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>984018.7099408599</v>
+      </c>
+      <c r="D6" t="n">
         <v>165781.63343531077</v>
       </c>
-      <c r="E6">
+      <c r="E6" t="n">
         <v>0.16847406635720813</v>
       </c>
       <c r="F6" t="s">
@@ -958,20 +651,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7">
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
-        <v>1999</v>
-      </c>
-      <c r="C7">
-        <v>552695.75742980966</v>
-      </c>
-      <c r="D7">
-        <v>99380.624370008911</v>
-      </c>
-      <c r="E7">
+      <c r="B7" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C7" t="n">
+        <v>552695.7574298097</v>
+      </c>
+      <c r="D7" t="n">
+        <v>99380.62437000891</v>
+      </c>
+      <c r="E7" t="n">
         <v>0.17981072413538454</v>
       </c>
       <c r="F7" t="s">
@@ -990,21 +683,21 @@
         <v>126</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8">
       <c r="A8" t="s">
         <v>15</v>
       </c>
-      <c r="B8">
-        <v>2001</v>
-      </c>
-      <c r="C8">
-        <v>1284660.1572940161</v>
-      </c>
-      <c r="D8">
+      <c r="B8" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1284660.157294016</v>
+      </c>
+      <c r="D8" t="n">
         <v>338968.20102694264</v>
       </c>
-      <c r="E8">
-        <v>0.26385826562951781</v>
+      <c r="E8" t="n">
+        <v>0.2638582656295178</v>
       </c>
       <c r="F8" t="s">
         <v>121</v>
@@ -1022,20 +715,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9">
-        <v>2003</v>
-      </c>
-      <c r="C9">
-        <v>965487.48196928215</v>
-      </c>
-      <c r="D9">
+      <c r="B9" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C9" t="n">
+        <v>965487.4819692821</v>
+      </c>
+      <c r="D9" t="n">
         <v>162682.63229057196</v>
       </c>
-      <c r="E9">
+      <c r="E9" t="n">
         <v>0.1684979197853006</v>
       </c>
       <c r="F9" t="s">
@@ -1054,20 +747,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10">
-        <v>2005</v>
-      </c>
-      <c r="C10">
+      <c r="B10" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C10" t="n">
         <v>1487568.0762175727</v>
       </c>
-      <c r="D10">
+      <c r="D10" t="n">
         <v>233497.68420472936</v>
       </c>
-      <c r="E10">
+      <c r="E10" t="n">
         <v>0.15696604944524087</v>
       </c>
       <c r="F10" t="s">
@@ -1086,20 +779,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B11">
-        <v>2007</v>
-      </c>
-      <c r="C11">
+      <c r="B11" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C11" t="n">
         <v>1397525.3597046805</v>
       </c>
-      <c r="D11">
+      <c r="D11" t="n">
         <v>242693.7712242112</v>
       </c>
-      <c r="E11">
+      <c r="E11" t="n">
         <v>0.173659654573636</v>
       </c>
       <c r="F11" t="s">
@@ -1118,21 +811,21 @@
         <v>126</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" t="s">
         <v>19</v>
       </c>
-      <c r="B12">
-        <v>2009</v>
-      </c>
-      <c r="C12">
+      <c r="B12" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C12" t="n">
         <v>1325088.8250739553</v>
       </c>
-      <c r="D12">
+      <c r="D12" t="n">
         <v>205902.994113016</v>
       </c>
-      <c r="E12">
-        <v>0.15538806925001741</v>
+      <c r="E12" t="n">
+        <v>0.1553880692500174</v>
       </c>
       <c r="F12" t="s">
         <v>121</v>
@@ -1150,20 +843,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" t="s">
         <v>20</v>
       </c>
-      <c r="B13">
-        <v>2011</v>
-      </c>
-      <c r="C13">
+      <c r="B13" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C13" t="n">
         <v>1792724.8037433089</v>
       </c>
-      <c r="D13">
-        <v>309780.23955103068</v>
-      </c>
-      <c r="E13">
+      <c r="D13" t="n">
+        <v>309780.2395510307</v>
+      </c>
+      <c r="E13" t="n">
         <v>0.17279854604800043</v>
       </c>
       <c r="F13" t="s">
@@ -1182,20 +875,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" t="s">
         <v>21</v>
       </c>
-      <c r="B14">
-        <v>2013</v>
-      </c>
-      <c r="C14">
+      <c r="B14" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C14" t="n">
         <v>2722636.1992887775</v>
       </c>
-      <c r="D14">
-        <v>507636.24352771102</v>
-      </c>
-      <c r="E14">
+      <c r="D14" t="n">
+        <v>507636.243527711</v>
+      </c>
+      <c r="E14" t="n">
         <v>0.18645026598130102</v>
       </c>
       <c r="F14" t="s">
@@ -1214,20 +907,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" t="s">
         <v>22</v>
       </c>
-      <c r="B15">
-        <v>2015</v>
-      </c>
-      <c r="C15">
-        <v>2989883.7250751639</v>
-      </c>
-      <c r="D15">
+      <c r="B15" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C15" t="n">
+        <v>2989883.725075164</v>
+      </c>
+      <c r="D15" t="n">
         <v>491999.6071709239</v>
       </c>
-      <c r="E15">
+      <c r="E15" t="n">
         <v>0.1645547627971905</v>
       </c>
       <c r="F15" t="s">
@@ -1246,20 +939,20 @@
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" t="s">
         <v>23</v>
       </c>
-      <c r="B16">
-        <v>1984</v>
-      </c>
-      <c r="C16">
+      <c r="B16" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C16" t="n">
         <v>474427.03254442697</v>
       </c>
-      <c r="D16">
+      <c r="D16" t="n">
         <v>74766.5503175669</v>
       </c>
-      <c r="E16">
+      <c r="E16" t="n">
         <v>0.15759336038796545</v>
       </c>
       <c r="F16" t="s">
@@ -1278,20 +971,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" t="s">
         <v>24</v>
       </c>
-      <c r="B17">
-        <v>1987</v>
-      </c>
-      <c r="C17">
-        <v>420679.44358645083</v>
-      </c>
-      <c r="D17">
-        <v>76898.729326280227</v>
-      </c>
-      <c r="E17">
+      <c r="B17" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C17" t="n">
+        <v>420679.4435864508</v>
+      </c>
+      <c r="D17" t="n">
+        <v>76898.72932628023</v>
+      </c>
+      <c r="E17" t="n">
         <v>0.18279649861350383</v>
       </c>
       <c r="F17" t="s">
@@ -1310,21 +1003,21 @@
         <v>127</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" t="s">
         <v>25</v>
       </c>
-      <c r="B18">
-        <v>1990</v>
-      </c>
-      <c r="C18">
-        <v>475261.97587105021</v>
-      </c>
-      <c r="D18">
-        <v>78941.490956288428</v>
-      </c>
-      <c r="E18">
-        <v>0.16610100316063811</v>
+      <c r="B18" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C18" t="n">
+        <v>475261.9758710502</v>
+      </c>
+      <c r="D18" t="n">
+        <v>78941.49095628843</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.1661010031606381</v>
       </c>
       <c r="F18" t="s">
         <v>121</v>
@@ -1342,20 +1035,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" t="s">
         <v>26</v>
       </c>
-      <c r="B19">
-        <v>1993</v>
-      </c>
-      <c r="C19">
-        <v>679035.28835818137</v>
-      </c>
-      <c r="D19">
+      <c r="B19" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C19" t="n">
+        <v>679035.2883581814</v>
+      </c>
+      <c r="D19" t="n">
         <v>113639.66006396255</v>
       </c>
-      <c r="E19">
+      <c r="E19" t="n">
         <v>0.16735457201160842</v>
       </c>
       <c r="F19" t="s">
@@ -1374,20 +1067,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B20">
-        <v>1996</v>
-      </c>
-      <c r="C20">
-        <v>889854.02490792971</v>
-      </c>
-      <c r="D20">
+      <c r="B20" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C20" t="n">
+        <v>889854.0249079297</v>
+      </c>
+      <c r="D20" t="n">
         <v>142327.47143913282</v>
       </c>
-      <c r="E20">
+      <c r="E20" t="n">
         <v>0.1599447408847299</v>
       </c>
       <c r="F20" t="s">
@@ -1406,20 +1099,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" t="s">
         <v>28</v>
       </c>
-      <c r="B21">
-        <v>1999</v>
-      </c>
-      <c r="C21">
-        <v>538342.02033238462</v>
-      </c>
-      <c r="D21">
-        <v>92790.912271905123</v>
-      </c>
-      <c r="E21">
+      <c r="B21" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C21" t="n">
+        <v>538342.0203323846</v>
+      </c>
+      <c r="D21" t="n">
+        <v>92790.91227190512</v>
+      </c>
+      <c r="E21" t="n">
         <v>0.1723642382859393</v>
       </c>
       <c r="F21" t="s">
@@ -1438,21 +1131,21 @@
         <v>127</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" t="s">
         <v>29</v>
       </c>
-      <c r="B22">
-        <v>2001</v>
-      </c>
-      <c r="C22">
+      <c r="B22" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C22" t="n">
         <v>1077333.4759203026</v>
       </c>
-      <c r="D22">
+      <c r="D22" t="n">
         <v>267973.59187099367</v>
       </c>
-      <c r="E22">
-        <v>0.24873783082074899</v>
+      <c r="E22" t="n">
+        <v>0.248737830820749</v>
       </c>
       <c r="F22" t="s">
         <v>121</v>
@@ -1470,20 +1163,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23">
       <c r="A23" t="s">
         <v>30</v>
       </c>
-      <c r="B23">
-        <v>2003</v>
-      </c>
-      <c r="C23">
-        <v>861997.96497598593</v>
-      </c>
-      <c r="D23">
-        <v>139547.79422559281</v>
-      </c>
-      <c r="E23">
+      <c r="B23" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C23" t="n">
+        <v>861997.9649759859</v>
+      </c>
+      <c r="D23" t="n">
+        <v>139547.7942255928</v>
+      </c>
+      <c r="E23" t="n">
         <v>0.16188877456280354</v>
       </c>
       <c r="F23" t="s">
@@ -1502,21 +1195,21 @@
         <v>127</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24">
       <c r="A24" t="s">
         <v>31</v>
       </c>
-      <c r="B24">
-        <v>2005</v>
-      </c>
-      <c r="C24">
-        <v>1324821.7660389021</v>
-      </c>
-      <c r="D24">
+      <c r="B24" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1324821.766038902</v>
+      </c>
+      <c r="D24" t="n">
         <v>195911.08636678924</v>
       </c>
-      <c r="E24">
-        <v>0.14787731556716929</v>
+      <c r="E24" t="n">
+        <v>0.1478773155671693</v>
       </c>
       <c r="F24" t="s">
         <v>121</v>
@@ -1534,20 +1227,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="25">
       <c r="A25" t="s">
         <v>32</v>
       </c>
-      <c r="B25">
-        <v>2007</v>
-      </c>
-      <c r="C25">
+      <c r="B25" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C25" t="n">
         <v>1203572.5993443127</v>
       </c>
-      <c r="D25">
-        <v>195566.70267951521</v>
-      </c>
-      <c r="E25">
+      <c r="D25" t="n">
+        <v>195566.7026795152</v>
+      </c>
+      <c r="E25" t="n">
         <v>0.16248849698477422</v>
       </c>
       <c r="F25" t="s">
@@ -1566,20 +1259,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="26">
       <c r="A26" t="s">
         <v>33</v>
       </c>
-      <c r="B26">
-        <v>2009</v>
-      </c>
-      <c r="C26">
+      <c r="B26" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C26" t="n">
         <v>1187511.8011958946</v>
       </c>
-      <c r="D26">
+      <c r="D26" t="n">
         <v>174572.54289303577</v>
       </c>
-      <c r="E26">
+      <c r="E26" t="n">
         <v>0.14700699623972655</v>
       </c>
       <c r="F26" t="s">
@@ -1598,20 +1291,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="27">
       <c r="A27" t="s">
         <v>34</v>
       </c>
-      <c r="B27">
-        <v>2011</v>
-      </c>
-      <c r="C27">
+      <c r="B27" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C27" t="n">
         <v>1543647.4331165375</v>
       </c>
-      <c r="D27">
+      <c r="D27" t="n">
         <v>251399.68073616424</v>
       </c>
-      <c r="E27">
+      <c r="E27" t="n">
         <v>0.16286081610526984</v>
       </c>
       <c r="F27" t="s">
@@ -1630,21 +1323,21 @@
         <v>127</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="28">
       <c r="A28" t="s">
         <v>35</v>
       </c>
-      <c r="B28">
-        <v>2013</v>
-      </c>
-      <c r="C28">
+      <c r="B28" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C28" t="n">
         <v>2418425.4555728254</v>
       </c>
-      <c r="D28">
+      <c r="D28" t="n">
         <v>431742.92524845706</v>
       </c>
-      <c r="E28">
-        <v>0.17852232089832801</v>
+      <c r="E28" t="n">
+        <v>0.178522320898328</v>
       </c>
       <c r="F28" t="s">
         <v>121</v>
@@ -1662,20 +1355,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="29">
       <c r="A29" t="s">
         <v>36</v>
       </c>
-      <c r="B29">
-        <v>2015</v>
-      </c>
-      <c r="C29">
-        <v>2840842.4545869431</v>
-      </c>
-      <c r="D29">
+      <c r="B29" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C29" t="n">
+        <v>2840842.454586943</v>
+      </c>
+      <c r="D29" t="n">
         <v>448503.39512585686</v>
       </c>
-      <c r="E29">
+      <c r="E29" t="n">
         <v>0.15787689824252116</v>
       </c>
       <c r="F29" t="s">
@@ -1694,20 +1387,20 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="30">
       <c r="A30" t="s">
         <v>37</v>
       </c>
-      <c r="B30">
-        <v>1984</v>
-      </c>
-      <c r="C30">
+      <c r="B30" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C30" t="n">
         <v>431068.1160869326</v>
       </c>
-      <c r="D30">
-        <v>68550.759051277113</v>
-      </c>
-      <c r="E30">
+      <c r="D30" t="n">
+        <v>68550.75905127711</v>
+      </c>
+      <c r="E30" t="n">
         <v>0.15902535235858786</v>
       </c>
       <c r="F30" t="s">
@@ -1726,20 +1419,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="31">
       <c r="A31" t="s">
         <v>38</v>
       </c>
-      <c r="B31">
-        <v>1987</v>
-      </c>
-      <c r="C31">
+      <c r="B31" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C31" t="n">
         <v>417188.8945729679</v>
       </c>
-      <c r="D31">
+      <c r="D31" t="n">
         <v>78482.63368709835</v>
       </c>
-      <c r="E31">
+      <c r="E31" t="n">
         <v>0.18812253803503737</v>
       </c>
       <c r="F31" t="s">
@@ -1758,21 +1451,21 @@
         <v>128</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="32">
       <c r="A32" t="s">
         <v>39</v>
       </c>
-      <c r="B32">
-        <v>1990</v>
-      </c>
-      <c r="C32">
-        <v>435831.69295209611</v>
-      </c>
-      <c r="D32">
-        <v>71948.736985885727</v>
-      </c>
-      <c r="E32">
-        <v>0.16508376547502221</v>
+      <c r="B32" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C32" t="n">
+        <v>435831.6929520961</v>
+      </c>
+      <c r="D32" t="n">
+        <v>71948.73698588573</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0.1650837654750222</v>
       </c>
       <c r="F32" t="s">
         <v>121</v>
@@ -1790,20 +1483,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33">
       <c r="A33" t="s">
         <v>40</v>
       </c>
-      <c r="B33">
-        <v>1993</v>
-      </c>
-      <c r="C33">
-        <v>633344.14388052106</v>
-      </c>
-      <c r="D33">
+      <c r="B33" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C33" t="n">
+        <v>633344.1438805211</v>
+      </c>
+      <c r="D33" t="n">
         <v>105627.55654971157</v>
       </c>
-      <c r="E33">
+      <c r="E33" t="n">
         <v>0.16677750567413152</v>
       </c>
       <c r="F33" t="s">
@@ -1822,21 +1515,21 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34">
       <c r="A34" t="s">
         <v>41</v>
       </c>
-      <c r="B34">
-        <v>1996</v>
-      </c>
-      <c r="C34">
-        <v>848285.74541709141</v>
-      </c>
-      <c r="D34">
+      <c r="B34" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C34" t="n">
+        <v>848285.7454170914</v>
+      </c>
+      <c r="D34" t="n">
         <v>138853.96117623523</v>
       </c>
-      <c r="E34">
-        <v>0.16368772188664149</v>
+      <c r="E34" t="n">
+        <v>0.1636877218866415</v>
       </c>
       <c r="F34" t="s">
         <v>121</v>
@@ -1854,20 +1547,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35">
       <c r="A35" t="s">
         <v>42</v>
       </c>
-      <c r="B35">
-        <v>1999</v>
-      </c>
-      <c r="C35">
+      <c r="B35" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C35" t="n">
         <v>523950.71790911694</v>
       </c>
-      <c r="D35">
+      <c r="D35" t="n">
         <v>91588.14666112815</v>
       </c>
-      <c r="E35">
+      <c r="E35" t="n">
         <v>0.17480297961346583</v>
       </c>
       <c r="F35" t="s">
@@ -1886,20 +1579,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36">
       <c r="A36" t="s">
         <v>43</v>
       </c>
-      <c r="B36">
-        <v>2001</v>
-      </c>
-      <c r="C36">
+      <c r="B36" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C36" t="n">
         <v>1029391.763157683</v>
       </c>
-      <c r="D36">
+      <c r="D36" t="n">
         <v>264056.30551109323</v>
       </c>
-      <c r="E36">
+      <c r="E36" t="n">
         <v>0.2565168237805735</v>
       </c>
       <c r="F36" t="s">
@@ -1918,20 +1611,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37">
       <c r="A37" t="s">
         <v>44</v>
       </c>
-      <c r="B37">
-        <v>2003</v>
-      </c>
-      <c r="C37">
-        <v>869153.95531629235</v>
-      </c>
-      <c r="D37">
+      <c r="B37" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C37" t="n">
+        <v>869153.9553162924</v>
+      </c>
+      <c r="D37" t="n">
         <v>142746.69767092084</v>
       </c>
-      <c r="E37">
+      <c r="E37" t="n">
         <v>0.16423637814427725</v>
       </c>
       <c r="F37" t="s">
@@ -1950,20 +1643,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38">
       <c r="A38" t="s">
         <v>45</v>
       </c>
-      <c r="B38">
-        <v>2005</v>
-      </c>
-      <c r="C38">
+      <c r="B38" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C38" t="n">
         <v>1259888.7519379575</v>
       </c>
-      <c r="D38">
+      <c r="D38" t="n">
         <v>186126.8374092236</v>
       </c>
-      <c r="E38">
+      <c r="E38" t="n">
         <v>0.14773275586667775</v>
       </c>
       <c r="F38" t="s">
@@ -1982,20 +1675,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39">
       <c r="A39" t="s">
         <v>46</v>
       </c>
-      <c r="B39">
-        <v>2007</v>
-      </c>
-      <c r="C39">
+      <c r="B39" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C39" t="n">
         <v>1185865.2896128064</v>
       </c>
-      <c r="D39">
+      <c r="D39" t="n">
         <v>197028.00839663818</v>
       </c>
-      <c r="E39">
+      <c r="E39" t="n">
         <v>0.16614704058078067</v>
       </c>
       <c r="F39" t="s">
@@ -2014,20 +1707,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40">
       <c r="A40" t="s">
         <v>47</v>
       </c>
-      <c r="B40">
-        <v>2009</v>
-      </c>
-      <c r="C40">
+      <c r="B40" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C40" t="n">
         <v>1068148.2080192536</v>
       </c>
-      <c r="D40">
+      <c r="D40" t="n">
         <v>157822.04267280936</v>
       </c>
-      <c r="E40">
+      <c r="E40" t="n">
         <v>0.14775294428988509</v>
       </c>
       <c r="F40" t="s">
@@ -2046,20 +1739,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41">
       <c r="A41" t="s">
         <v>48</v>
       </c>
-      <c r="B41">
-        <v>2011</v>
-      </c>
-      <c r="C41">
+      <c r="B41" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C41" t="n">
         <v>1502430.6576236687</v>
       </c>
-      <c r="D41">
-        <v>247591.25172703291</v>
-      </c>
-      <c r="E41">
+      <c r="D41" t="n">
+        <v>247591.2517270329</v>
+      </c>
+      <c r="E41" t="n">
         <v>0.16479379628650387</v>
       </c>
       <c r="F41" t="s">
@@ -2078,20 +1771,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42">
       <c r="A42" t="s">
         <v>49</v>
       </c>
-      <c r="B42">
-        <v>2013</v>
-      </c>
-      <c r="C42">
+      <c r="B42" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C42" t="n">
         <v>2140815.195833141</v>
       </c>
-      <c r="D42">
+      <c r="D42" t="n">
         <v>380589.75845871016</v>
       </c>
-      <c r="E42">
+      <c r="E42" t="n">
         <v>0.17777796009645572</v>
       </c>
       <c r="F42" t="s">
@@ -2110,20 +1803,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43">
       <c r="A43" t="s">
         <v>50</v>
       </c>
-      <c r="B43">
-        <v>2015</v>
-      </c>
-      <c r="C43">
-        <v>2646859.4060347392</v>
-      </c>
-      <c r="D43">
-        <v>426481.19590961363</v>
-      </c>
-      <c r="E43">
+      <c r="B43" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C43" t="n">
+        <v>2646859.406034739</v>
+      </c>
+      <c r="D43" t="n">
+        <v>426481.1959096136</v>
+      </c>
+      <c r="E43" t="n">
         <v>0.16112725705689265</v>
       </c>
       <c r="F43" t="s">
@@ -2142,20 +1835,20 @@
         <v>128</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44">
       <c r="A44" t="s">
         <v>51</v>
       </c>
-      <c r="B44">
-        <v>1984</v>
-      </c>
-      <c r="C44">
-        <v>422011.26274257741</v>
-      </c>
-      <c r="D44">
-        <v>66434.513421661948</v>
-      </c>
-      <c r="E44">
+      <c r="B44" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C44" t="n">
+        <v>422011.2627425774</v>
+      </c>
+      <c r="D44" t="n">
+        <v>66434.51342166195</v>
+      </c>
+      <c r="E44" t="n">
         <v>0.15742355545185135</v>
       </c>
       <c r="F44" t="s">
@@ -2174,20 +1867,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45">
       <c r="A45" t="s">
         <v>52</v>
       </c>
-      <c r="B45">
-        <v>1987</v>
-      </c>
-      <c r="C45">
-        <v>413748.97472745151</v>
-      </c>
-      <c r="D45">
+      <c r="B45" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C45" t="n">
+        <v>413748.9747274515</v>
+      </c>
+      <c r="D45" t="n">
         <v>78205.2446753283</v>
       </c>
-      <c r="E45">
+      <c r="E45" t="n">
         <v>0.18901616548257158</v>
       </c>
       <c r="F45" t="s">
@@ -2206,20 +1899,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46">
       <c r="A46" t="s">
         <v>53</v>
       </c>
-      <c r="B46">
-        <v>1990</v>
-      </c>
-      <c r="C46">
+      <c r="B46" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C46" t="n">
         <v>411354.09450385923</v>
       </c>
-      <c r="D46">
-        <v>67576.292874794861</v>
-      </c>
-      <c r="E46">
+      <c r="D46" t="n">
+        <v>67576.29287479486</v>
+      </c>
+      <c r="E46" t="n">
         <v>0.16427767166460253</v>
       </c>
       <c r="F46" t="s">
@@ -2238,21 +1931,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47">
       <c r="A47" t="s">
         <v>54</v>
       </c>
-      <c r="B47">
-        <v>1993</v>
-      </c>
-      <c r="C47">
-        <v>613157.90576196928</v>
-      </c>
-      <c r="D47">
+      <c r="B47" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C47" t="n">
+        <v>613157.9057619693</v>
+      </c>
+      <c r="D47" t="n">
         <v>102229.42303754785</v>
       </c>
-      <c r="E47">
-        <v>0.16672609465991911</v>
+      <c r="E47" t="n">
+        <v>0.1667260946599191</v>
       </c>
       <c r="F47" t="s">
         <v>121</v>
@@ -2270,20 +1963,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48">
       <c r="A48" t="s">
         <v>55</v>
       </c>
-      <c r="B48">
-        <v>1996</v>
-      </c>
-      <c r="C48">
-        <v>812870.26794112311</v>
-      </c>
-      <c r="D48">
+      <c r="B48" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C48" t="n">
+        <v>812870.2679411231</v>
+      </c>
+      <c r="D48" t="n">
         <v>131375.88039351895</v>
       </c>
-      <c r="E48">
+      <c r="E48" t="n">
         <v>0.16161973881302621</v>
       </c>
       <c r="F48" t="s">
@@ -2302,20 +1995,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="49">
       <c r="A49" t="s">
         <v>56</v>
       </c>
-      <c r="B49">
-        <v>1999</v>
-      </c>
-      <c r="C49">
+      <c r="B49" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C49" t="n">
         <v>523110.58720579423</v>
       </c>
-      <c r="D49">
-        <v>90334.112821695817</v>
-      </c>
-      <c r="E49">
+      <c r="D49" t="n">
+        <v>90334.11282169582</v>
+      </c>
+      <c r="E49" t="n">
         <v>0.17268645489325174</v>
       </c>
       <c r="F49" t="s">
@@ -2334,20 +2027,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="50">
       <c r="A50" t="s">
         <v>57</v>
       </c>
-      <c r="B50">
-        <v>2001</v>
-      </c>
-      <c r="C50">
+      <c r="B50" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C50" t="n">
         <v>1014444.9647673602</v>
       </c>
-      <c r="D50">
+      <c r="D50" t="n">
         <v>260304.03272863722</v>
       </c>
-      <c r="E50">
+      <c r="E50" t="n">
         <v>0.25659749101158186</v>
       </c>
       <c r="F50" t="s">
@@ -2366,20 +2059,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="51">
       <c r="A51" t="s">
         <v>58</v>
       </c>
-      <c r="B51">
-        <v>2003</v>
-      </c>
-      <c r="C51">
-        <v>819887.82833270403</v>
-      </c>
-      <c r="D51">
-        <v>134442.15417835541</v>
-      </c>
-      <c r="E51">
+      <c r="B51" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C51" t="n">
+        <v>819887.828332704</v>
+      </c>
+      <c r="D51" t="n">
+        <v>134442.1541783554</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.16397627764733672</v>
       </c>
       <c r="F51" t="s">
@@ -2398,20 +2091,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="52">
       <c r="A52" t="s">
         <v>59</v>
       </c>
-      <c r="B52">
-        <v>2005</v>
-      </c>
-      <c r="C52">
+      <c r="B52" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C52" t="n">
         <v>1248448.7691745015</v>
       </c>
-      <c r="D52">
+      <c r="D52" t="n">
         <v>184486.56425966407</v>
       </c>
-      <c r="E52">
+      <c r="E52" t="n">
         <v>0.14777263498096935</v>
       </c>
       <c r="F52" t="s">
@@ -2430,20 +2123,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="53">
       <c r="A53" t="s">
         <v>60</v>
       </c>
-      <c r="B53">
-        <v>2007</v>
-      </c>
-      <c r="C53">
+      <c r="B53" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C53" t="n">
         <v>1167333.3670408751</v>
       </c>
-      <c r="D53">
+      <c r="D53" t="n">
         <v>191421.77233299828</v>
       </c>
-      <c r="E53">
+      <c r="E53" t="n">
         <v>0.16398209606416184</v>
       </c>
       <c r="F53" t="s">
@@ -2462,20 +2155,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="54">
       <c r="A54" t="s">
         <v>61</v>
       </c>
-      <c r="B54">
-        <v>2009</v>
-      </c>
-      <c r="C54">
+      <c r="B54" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C54" t="n">
         <v>1097487.3149838073</v>
       </c>
-      <c r="D54">
+      <c r="D54" t="n">
         <v>161481.14868853902</v>
       </c>
-      <c r="E54">
+      <c r="E54" t="n">
         <v>0.14713714362240402</v>
       </c>
       <c r="F54" t="s">
@@ -2494,20 +2187,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="55">
       <c r="A55" t="s">
         <v>62</v>
       </c>
-      <c r="B55">
-        <v>2011</v>
-      </c>
-      <c r="C55">
+      <c r="B55" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C55" t="n">
         <v>1432179.1808930982</v>
       </c>
-      <c r="D55">
+      <c r="D55" t="n">
         <v>232207.43816873123</v>
       </c>
-      <c r="E55">
+      <c r="E55" t="n">
         <v>0.16213574479132428</v>
       </c>
       <c r="F55" t="s">
@@ -2526,21 +2219,21 @@
         <v>129</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="56">
       <c r="A56" t="s">
         <v>63</v>
       </c>
-      <c r="B56">
-        <v>2013</v>
-      </c>
-      <c r="C56">
-        <v>2189958.9481585468</v>
-      </c>
-      <c r="D56">
+      <c r="B56" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C56" t="n">
+        <v>2189958.948158547</v>
+      </c>
+      <c r="D56" t="n">
         <v>390893.31280137866</v>
       </c>
-      <c r="E56">
-        <v>0.17849344305292389</v>
+      <c r="E56" t="n">
+        <v>0.1784934430529239</v>
       </c>
       <c r="F56" t="s">
         <v>121</v>
@@ -2558,20 +2251,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="57">
       <c r="A57" t="s">
         <v>64</v>
       </c>
-      <c r="B57">
-        <v>2015</v>
-      </c>
-      <c r="C57">
-        <v>2578610.7978211311</v>
-      </c>
-      <c r="D57">
-        <v>409574.37838783063</v>
-      </c>
-      <c r="E57">
+      <c r="B57" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C57" t="n">
+        <v>2578610.797821131</v>
+      </c>
+      <c r="D57" t="n">
+        <v>409574.3783878306</v>
+      </c>
+      <c r="E57" t="n">
         <v>0.1588352839962944</v>
       </c>
       <c r="F57" t="s">
@@ -2590,20 +2283,20 @@
         <v>129</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="58">
       <c r="A58" t="s">
         <v>65</v>
       </c>
-      <c r="B58">
-        <v>1984</v>
-      </c>
-      <c r="C58">
+      <c r="B58" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C58" t="n">
         <v>369401.98466360266</v>
       </c>
-      <c r="D58">
+      <c r="D58" t="n">
         <v>57272.05970717984</v>
       </c>
-      <c r="E58">
+      <c r="E58" t="n">
         <v>0.1550399350434862</v>
       </c>
       <c r="F58" t="s">
@@ -2622,20 +2315,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="59">
       <c r="A59" t="s">
         <v>66</v>
       </c>
-      <c r="B59">
-        <v>1987</v>
-      </c>
-      <c r="C59">
-        <v>371155.74644349387</v>
-      </c>
-      <c r="D59">
-        <v>66801.158107236872</v>
-      </c>
-      <c r="E59">
+      <c r="B59" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C59" t="n">
+        <v>371155.7464434939</v>
+      </c>
+      <c r="D59" t="n">
+        <v>66801.15810723687</v>
+      </c>
+      <c r="E59" t="n">
         <v>0.17998147340393375</v>
       </c>
       <c r="F59" t="s">
@@ -2654,20 +2347,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="60">
       <c r="A60" t="s">
         <v>67</v>
       </c>
-      <c r="B60">
-        <v>1990</v>
-      </c>
-      <c r="C60">
+      <c r="B60" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C60" t="n">
         <v>382849.35711037944</v>
       </c>
-      <c r="D60">
+      <c r="D60" t="n">
         <v>61555.4240690566</v>
       </c>
-      <c r="E60">
+      <c r="E60" t="n">
         <v>0.16078236237264865</v>
       </c>
       <c r="F60" t="s">
@@ -2686,21 +2379,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="61">
       <c r="A61" t="s">
         <v>68</v>
       </c>
-      <c r="B61">
-        <v>1993</v>
-      </c>
-      <c r="C61">
-        <v>567008.81477547577</v>
-      </c>
-      <c r="D61">
-        <v>93472.586378977605</v>
-      </c>
-      <c r="E61">
-        <v>0.16485208685157901</v>
+      <c r="B61" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C61" t="n">
+        <v>567008.8147754758</v>
+      </c>
+      <c r="D61" t="n">
+        <v>93472.5863789776</v>
+      </c>
+      <c r="E61" t="n">
+        <v>0.164852086851579</v>
       </c>
       <c r="F61" t="s">
         <v>121</v>
@@ -2718,21 +2411,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="62">
       <c r="A62" t="s">
         <v>69</v>
       </c>
-      <c r="B62">
-        <v>1996</v>
-      </c>
-      <c r="C62">
-        <v>742449.80627519789</v>
-      </c>
-      <c r="D62">
+      <c r="B62" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C62" t="n">
+        <v>742449.8062751979</v>
+      </c>
+      <c r="D62" t="n">
         <v>116839.99146199053</v>
       </c>
-      <c r="E62">
-        <v>0.15737089628747561</v>
+      <c r="E62" t="n">
+        <v>0.1573708962874756</v>
       </c>
       <c r="F62" t="s">
         <v>121</v>
@@ -2750,20 +2443,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="63">
       <c r="A63" t="s">
         <v>70</v>
       </c>
-      <c r="B63">
-        <v>1999</v>
-      </c>
-      <c r="C63">
-        <v>477297.98235420563</v>
-      </c>
-      <c r="D63">
-        <v>80529.344470799901</v>
-      </c>
-      <c r="E63">
+      <c r="B63" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C63" t="n">
+        <v>477297.9823542056</v>
+      </c>
+      <c r="D63" t="n">
+        <v>80529.3444707999</v>
+      </c>
+      <c r="E63" t="n">
         <v>0.16871922247313964</v>
       </c>
       <c r="F63" t="s">
@@ -2782,20 +2475,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="64">
       <c r="A64" t="s">
         <v>71</v>
       </c>
-      <c r="B64">
-        <v>2001</v>
-      </c>
-      <c r="C64">
-        <v>998143.78804678784</v>
-      </c>
-      <c r="D64">
+      <c r="B64" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C64" t="n">
+        <v>998143.7880467878</v>
+      </c>
+      <c r="D64" t="n">
         <v>246238.15146364766</v>
       </c>
-      <c r="E64">
+      <c r="E64" t="n">
         <v>0.2466960716606747</v>
       </c>
       <c r="F64" t="s">
@@ -2814,20 +2507,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="65" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="65">
       <c r="A65" t="s">
         <v>72</v>
       </c>
-      <c r="B65">
-        <v>2003</v>
-      </c>
-      <c r="C65">
-        <v>839455.94072383491</v>
-      </c>
-      <c r="D65">
+      <c r="B65" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C65" t="n">
+        <v>839455.9407238349</v>
+      </c>
+      <c r="D65" t="n">
         <v>136636.22165170425</v>
       </c>
-      <c r="E65">
+      <c r="E65" t="n">
         <v>0.1627675915115776</v>
       </c>
       <c r="F65" t="s">
@@ -2846,21 +2539,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="66">
       <c r="A66" t="s">
         <v>73</v>
       </c>
-      <c r="B66">
-        <v>2005</v>
-      </c>
-      <c r="C66">
+      <c r="B66" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C66" t="n">
         <v>1205025.836167396</v>
       </c>
-      <c r="D66">
+      <c r="D66" t="n">
         <v>174908.6057504669</v>
       </c>
-      <c r="E66">
-        <v>0.14514925780078419</v>
+      <c r="E66" t="n">
+        <v>0.1451492578007842</v>
       </c>
       <c r="F66" t="s">
         <v>121</v>
@@ -2878,20 +2571,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="67">
       <c r="A67" t="s">
         <v>74</v>
       </c>
-      <c r="B67">
-        <v>2007</v>
-      </c>
-      <c r="C67">
-        <v>1135328.8240411461</v>
-      </c>
-      <c r="D67">
-        <v>184831.62458080481</v>
-      </c>
-      <c r="E67">
+      <c r="B67" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C67" t="n">
+        <v>1135328.824041146</v>
+      </c>
+      <c r="D67" t="n">
+        <v>184831.6245808048</v>
+      </c>
+      <c r="E67" t="n">
         <v>0.16280008105749125</v>
       </c>
       <c r="F67" t="s">
@@ -2910,20 +2603,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="68" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="68">
       <c r="A68" t="s">
         <v>75</v>
       </c>
-      <c r="B68">
-        <v>2009</v>
-      </c>
-      <c r="C68">
+      <c r="B68" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C68" t="n">
         <v>1059468.2925717311</v>
       </c>
-      <c r="D68">
+      <c r="D68" t="n">
         <v>155261.16098529383</v>
       </c>
-      <c r="E68">
+      <c r="E68" t="n">
         <v>0.14654630258770288</v>
       </c>
       <c r="F68" t="s">
@@ -2942,20 +2635,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="69" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="69">
       <c r="A69" t="s">
         <v>76</v>
       </c>
-      <c r="B69">
-        <v>2011</v>
-      </c>
-      <c r="C69">
+      <c r="B69" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C69" t="n">
         <v>1433252.0660261535</v>
       </c>
-      <c r="D69">
+      <c r="D69" t="n">
         <v>234508.99138062095</v>
       </c>
-      <c r="E69">
+      <c r="E69" t="n">
         <v>0.16362020117704942</v>
       </c>
       <c r="F69" t="s">
@@ -2974,20 +2667,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="70" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="70">
       <c r="A70" t="s">
         <v>77</v>
       </c>
-      <c r="B70">
-        <v>2013</v>
-      </c>
-      <c r="C70">
+      <c r="B70" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C70" t="n">
         <v>2115766.225874092</v>
       </c>
-      <c r="D70">
+      <c r="D70" t="n">
         <v>377656.18296203145</v>
       </c>
-      <c r="E70">
+      <c r="E70" t="n">
         <v>0.17849617710293555</v>
       </c>
       <c r="F70" t="s">
@@ -3006,20 +2699,20 @@
         <v>130</v>
       </c>
     </row>
-    <row r="71" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="71">
       <c r="A71" t="s">
         <v>78</v>
       </c>
-      <c r="B71">
-        <v>2015</v>
-      </c>
-      <c r="C71">
-        <v>2478575.5927290861</v>
-      </c>
-      <c r="D71">
+      <c r="B71" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C71" t="n">
+        <v>2478575.592729086</v>
+      </c>
+      <c r="D71" t="n">
         <v>390710.74678239564</v>
       </c>
-      <c r="E71">
+      <c r="E71" t="n">
         <v>0.15763519495977754</v>
       </c>
       <c r="F71" t="s">
@@ -3038,21 +2731,21 @@
         <v>130</v>
       </c>
     </row>
-    <row r="72" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="72">
       <c r="A72" t="s">
         <v>79</v>
       </c>
-      <c r="B72">
-        <v>1984</v>
-      </c>
-      <c r="C72">
+      <c r="B72" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C72" t="n">
         <v>340201.75655266066</v>
       </c>
-      <c r="D72">
-        <v>52393.020689150108</v>
-      </c>
-      <c r="E72">
-        <v>0.15400573242201959</v>
+      <c r="D72" t="n">
+        <v>52393.02068915011</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.1540057324220196</v>
       </c>
       <c r="F72" t="s">
         <v>121</v>
@@ -3070,20 +2763,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="73" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="73">
       <c r="A73" t="s">
         <v>80</v>
       </c>
-      <c r="B73">
-        <v>1987</v>
-      </c>
-      <c r="C73">
-        <v>342568.67885827139</v>
-      </c>
-      <c r="D73">
-        <v>61310.864010623809</v>
-      </c>
-      <c r="E73">
+      <c r="B73" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C73" t="n">
+        <v>342568.6788582714</v>
+      </c>
+      <c r="D73" t="n">
+        <v>61310.86401062381</v>
+      </c>
+      <c r="E73" t="n">
         <v>0.17897393367941128</v>
       </c>
       <c r="F73" t="s">
@@ -3102,20 +2795,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="74">
       <c r="A74" t="s">
         <v>81</v>
       </c>
-      <c r="B74">
-        <v>1990</v>
-      </c>
-      <c r="C74">
+      <c r="B74" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C74" t="n">
         <v>338427.95813277713</v>
       </c>
-      <c r="D74">
+      <c r="D74" t="n">
         <v>53257.05659795391</v>
       </c>
-      <c r="E74">
+      <c r="E74" t="n">
         <v>0.15736600750065485</v>
       </c>
       <c r="F74" t="s">
@@ -3134,20 +2827,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="75" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="75">
       <c r="A75" t="s">
         <v>82</v>
       </c>
-      <c r="B75">
-        <v>1993</v>
-      </c>
-      <c r="C75">
+      <c r="B75" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C75" t="n">
         <v>474901.41173596424</v>
       </c>
-      <c r="D75">
-        <v>75989.628824003084</v>
-      </c>
-      <c r="E75">
+      <c r="D75" t="n">
+        <v>75989.62882400308</v>
+      </c>
+      <c r="E75" t="n">
         <v>0.16001137698502318</v>
       </c>
       <c r="F75" t="s">
@@ -3166,21 +2859,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="76" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="76">
       <c r="A76" t="s">
         <v>83</v>
       </c>
-      <c r="B76">
-        <v>1996</v>
-      </c>
-      <c r="C76">
-        <v>631889.12717596593</v>
-      </c>
-      <c r="D76">
-        <v>99136.257990066471</v>
-      </c>
-      <c r="E76">
-        <v>0.15688869095299279</v>
+      <c r="B76" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C76" t="n">
+        <v>631889.1271759659</v>
+      </c>
+      <c r="D76" t="n">
+        <v>99136.25799006647</v>
+      </c>
+      <c r="E76" t="n">
+        <v>0.1568886909529928</v>
       </c>
       <c r="F76" t="s">
         <v>121</v>
@@ -3198,21 +2891,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="77" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="77">
       <c r="A77" t="s">
         <v>84</v>
       </c>
-      <c r="B77">
-        <v>1999</v>
-      </c>
-      <c r="C77">
+      <c r="B77" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C77" t="n">
         <v>477782.73385954835</v>
       </c>
-      <c r="D77">
-        <v>80641.872392761783</v>
-      </c>
-      <c r="E77">
-        <v>0.16878356348571549</v>
+      <c r="D77" t="n">
+        <v>80641.87239276178</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.1687835634857155</v>
       </c>
       <c r="F77" t="s">
         <v>121</v>
@@ -3230,20 +2923,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="78" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="78">
       <c r="A78" t="s">
         <v>85</v>
       </c>
-      <c r="B78">
-        <v>2001</v>
-      </c>
-      <c r="C78">
-        <v>881485.95675127744</v>
-      </c>
-      <c r="D78">
-        <v>217554.13436939591</v>
-      </c>
-      <c r="E78">
+      <c r="B78" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C78" t="n">
+        <v>881485.9567512774</v>
+      </c>
+      <c r="D78" t="n">
+        <v>217554.1343693959</v>
+      </c>
+      <c r="E78" t="n">
         <v>0.24680385739915037</v>
       </c>
       <c r="F78" t="s">
@@ -3262,20 +2955,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="79" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="79">
       <c r="A79" t="s">
         <v>86</v>
       </c>
-      <c r="B79">
-        <v>2003</v>
-      </c>
-      <c r="C79">
-        <v>745224.79998401972</v>
-      </c>
-      <c r="D79">
+      <c r="B79" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C79" t="n">
+        <v>745224.7999840197</v>
+      </c>
+      <c r="D79" t="n">
         <v>118617.59072048993</v>
       </c>
-      <c r="E79">
+      <c r="E79" t="n">
         <v>0.15917021377044016</v>
       </c>
       <c r="F79" t="s">
@@ -3294,20 +2987,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="80" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="80">
       <c r="A80" t="s">
         <v>87</v>
       </c>
-      <c r="B80">
-        <v>2005</v>
-      </c>
-      <c r="C80">
+      <c r="B80" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C80" t="n">
         <v>1127007.4017308222</v>
       </c>
-      <c r="D80">
+      <c r="D80" t="n">
         <v>161610.15449929528</v>
       </c>
-      <c r="E80">
+      <c r="E80" t="n">
         <v>0.14339759814451933</v>
       </c>
       <c r="F80" t="s">
@@ -3326,21 +3019,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="81">
       <c r="A81" t="s">
         <v>88</v>
       </c>
-      <c r="B81">
-        <v>2007</v>
-      </c>
-      <c r="C81">
+      <c r="B81" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C81" t="n">
         <v>1125370.7582171564</v>
       </c>
-      <c r="D81">
+      <c r="D81" t="n">
         <v>182452.02022004698</v>
       </c>
-      <c r="E81">
-        <v>0.16212614277368689</v>
+      <c r="E81" t="n">
+        <v>0.1621261427736869</v>
       </c>
       <c r="F81" t="s">
         <v>121</v>
@@ -3358,21 +3051,21 @@
         <v>131</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="82">
       <c r="A82" t="s">
         <v>89</v>
       </c>
-      <c r="B82">
-        <v>2009</v>
-      </c>
-      <c r="C82">
+      <c r="B82" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C82" t="n">
         <v>1052573.8849252735</v>
       </c>
-      <c r="D82">
+      <c r="D82" t="n">
         <v>152563.20898103632</v>
       </c>
-      <c r="E82">
-        <v>0.14494299275899991</v>
+      <c r="E82" t="n">
+        <v>0.1449429927589999</v>
       </c>
       <c r="F82" t="s">
         <v>121</v>
@@ -3390,20 +3083,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="83" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="83">
       <c r="A83" t="s">
         <v>90</v>
       </c>
-      <c r="B83">
-        <v>2011</v>
-      </c>
-      <c r="C83">
+      <c r="B83" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C83" t="n">
         <v>1403342.7463995798</v>
       </c>
-      <c r="D83">
+      <c r="D83" t="n">
         <v>224718.23001158526</v>
       </c>
-      <c r="E83">
+      <c r="E83" t="n">
         <v>0.16013068125240465</v>
       </c>
       <c r="F83" t="s">
@@ -3422,20 +3115,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="84" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="84">
       <c r="A84" t="s">
         <v>91</v>
       </c>
-      <c r="B84">
-        <v>2013</v>
-      </c>
-      <c r="C84">
+      <c r="B84" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C84" t="n">
         <v>1947647.4219548283</v>
       </c>
-      <c r="D84">
-        <v>345888.75058802217</v>
-      </c>
-      <c r="E84">
+      <c r="D84" t="n">
+        <v>345888.7505880222</v>
+      </c>
+      <c r="E84" t="n">
         <v>0.17759310370501152</v>
       </c>
       <c r="F84" t="s">
@@ -3454,20 +3147,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="85" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="85">
       <c r="A85" t="s">
         <v>92</v>
       </c>
-      <c r="B85">
-        <v>2015</v>
-      </c>
-      <c r="C85">
+      <c r="B85" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C85" t="n">
         <v>2356248.1557635716</v>
       </c>
-      <c r="D85">
-        <v>371221.03861747228</v>
-      </c>
-      <c r="E85">
+      <c r="D85" t="n">
+        <v>371221.0386174723</v>
+      </c>
+      <c r="E85" t="n">
         <v>0.1575475137070923</v>
       </c>
       <c r="F85" t="s">
@@ -3486,20 +3179,20 @@
         <v>131</v>
       </c>
     </row>
-    <row r="86" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="86">
       <c r="A86" t="s">
         <v>93</v>
       </c>
-      <c r="B86">
-        <v>1984</v>
-      </c>
-      <c r="C86">
-        <v>327575.12048778782</v>
-      </c>
-      <c r="D86">
-        <v>50491.155319221281</v>
-      </c>
-      <c r="E86">
+      <c r="B86" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C86" t="n">
+        <v>327575.1204877878</v>
+      </c>
+      <c r="D86" t="n">
+        <v>50491.15531922128</v>
+      </c>
+      <c r="E86" t="n">
         <v>0.15413611157048668</v>
       </c>
       <c r="F86" t="s">
@@ -3518,21 +3211,21 @@
         <v>132</v>
       </c>
     </row>
-    <row r="87" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="87">
       <c r="A87" t="s">
         <v>94</v>
       </c>
-      <c r="B87">
-        <v>1987</v>
-      </c>
-      <c r="C87">
+      <c r="B87" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C87" t="n">
         <v>331577.91016923566</v>
       </c>
-      <c r="D87">
+      <c r="D87" t="n">
         <v>57882.544136540135</v>
       </c>
-      <c r="E87">
-        <v>0.17456694900754149</v>
+      <c r="E87" t="n">
+        <v>0.1745669490075415</v>
       </c>
       <c r="F87" t="s">
         <v>121</v>
@@ -3550,20 +3243,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="88" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="88">
       <c r="A88" t="s">
         <v>95</v>
       </c>
-      <c r="B88">
-        <v>1990</v>
-      </c>
-      <c r="C88">
+      <c r="B88" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C88" t="n">
         <v>333803.4979335884</v>
       </c>
-      <c r="D88">
+      <c r="D88" t="n">
         <v>52126.206805904614</v>
       </c>
-      <c r="E88">
+      <c r="E88" t="n">
         <v>0.15615836001896943</v>
       </c>
       <c r="F88" t="s">
@@ -3582,20 +3275,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="89" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="89">
       <c r="A89" t="s">
         <v>96</v>
       </c>
-      <c r="B89">
-        <v>1993</v>
-      </c>
-      <c r="C89">
-        <v>468822.63022435462</v>
-      </c>
-      <c r="D89">
-        <v>74037.918689071201</v>
-      </c>
-      <c r="E89">
+      <c r="B89" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C89" t="n">
+        <v>468822.6302243546</v>
+      </c>
+      <c r="D89" t="n">
+        <v>74037.9186890712</v>
+      </c>
+      <c r="E89" t="n">
         <v>0.15792309055908932</v>
       </c>
       <c r="F89" t="s">
@@ -3614,21 +3307,21 @@
         <v>132</v>
       </c>
     </row>
-    <row r="90" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="90">
       <c r="A90" t="s">
         <v>97</v>
       </c>
-      <c r="B90">
-        <v>1996</v>
-      </c>
-      <c r="C90">
-        <v>619073.94737658894</v>
-      </c>
-      <c r="D90">
-        <v>95050.820888914677</v>
-      </c>
-      <c r="E90">
-        <v>0.15353710375263829</v>
+      <c r="B90" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C90" t="n">
+        <v>619073.9473765889</v>
+      </c>
+      <c r="D90" t="n">
+        <v>95050.82088891468</v>
+      </c>
+      <c r="E90" t="n">
+        <v>0.1535371037526383</v>
       </c>
       <c r="F90" t="s">
         <v>121</v>
@@ -3646,20 +3339,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="91" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="91">
       <c r="A91" t="s">
         <v>98</v>
       </c>
-      <c r="B91">
-        <v>1999</v>
-      </c>
-      <c r="C91">
-        <v>465585.60817175527</v>
-      </c>
-      <c r="D91">
-        <v>76771.441535437712</v>
-      </c>
-      <c r="E91">
+      <c r="B91" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C91" t="n">
+        <v>465585.6081717553</v>
+      </c>
+      <c r="D91" t="n">
+        <v>76771.44153543771</v>
+      </c>
+      <c r="E91" t="n">
         <v>0.16489221356497902</v>
       </c>
       <c r="F91" t="s">
@@ -3678,20 +3371,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="92" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="92">
       <c r="A92" t="s">
         <v>99</v>
       </c>
-      <c r="B92">
-        <v>2001</v>
-      </c>
-      <c r="C92">
+      <c r="B92" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C92" t="n">
         <v>853805.3569865952</v>
       </c>
-      <c r="D92">
+      <c r="D92" t="n">
         <v>203661.7244605381</v>
       </c>
-      <c r="E92">
+      <c r="E92" t="n">
         <v>0.23853413754551508</v>
       </c>
       <c r="F92" t="s">
@@ -3710,20 +3403,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="93" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="93">
       <c r="A93" t="s">
         <v>100</v>
       </c>
-      <c r="B93">
-        <v>2003</v>
-      </c>
-      <c r="C93">
-        <v>699057.42713349382</v>
-      </c>
-      <c r="D93">
+      <c r="B93" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C93" t="n">
+        <v>699057.4271334938</v>
+      </c>
+      <c r="D93" t="n">
         <v>108779.30809902039</v>
       </c>
-      <c r="E93">
+      <c r="E93" t="n">
         <v>0.15560854355710552</v>
       </c>
       <c r="F93" t="s">
@@ -3742,20 +3435,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="94" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="94">
       <c r="A94" t="s">
         <v>101</v>
       </c>
-      <c r="B94">
-        <v>2005</v>
-      </c>
-      <c r="C94">
+      <c r="B94" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C94" t="n">
         <v>1046814.2695377726</v>
       </c>
-      <c r="D94">
+      <c r="D94" t="n">
         <v>148046.75224380186</v>
       </c>
-      <c r="E94">
+      <c r="E94" t="n">
         <v>0.14142599747820866</v>
       </c>
       <c r="F94" t="s">
@@ -3774,20 +3467,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="95" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="95">
       <c r="A95" t="s">
         <v>102</v>
       </c>
-      <c r="B95">
-        <v>2007</v>
-      </c>
-      <c r="C95" s="3">
+      <c r="B95" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C95" t="n">
         <v>1061249.3673510056</v>
       </c>
-      <c r="D95">
+      <c r="D95" t="n">
         <v>170680.05271289448</v>
       </c>
-      <c r="E95">
+      <c r="E95" t="n">
         <v>0.16082935638296827</v>
       </c>
       <c r="F95" t="s">
@@ -3806,20 +3499,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="96" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="96">
       <c r="A96" t="s">
         <v>103</v>
       </c>
-      <c r="B96">
-        <v>2009</v>
-      </c>
-      <c r="C96" s="3">
+      <c r="B96" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C96" t="n">
         <v>1027719.5211325879</v>
       </c>
-      <c r="D96">
+      <c r="D96" t="n">
         <v>148569.78123771076</v>
       </c>
-      <c r="E96">
+      <c r="E96" t="n">
         <v>0.14456257586114638</v>
       </c>
       <c r="F96" t="s">
@@ -3838,20 +3531,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="97">
       <c r="A97" t="s">
         <v>104</v>
       </c>
-      <c r="B97">
-        <v>2011</v>
-      </c>
-      <c r="C97" s="3">
+      <c r="B97" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C97" t="n">
         <v>1309415.106768115</v>
       </c>
-      <c r="D97">
+      <c r="D97" t="n">
         <v>206334.94814309967</v>
       </c>
-      <c r="E97">
+      <c r="E97" t="n">
         <v>0.15757794993855959</v>
       </c>
       <c r="F97" t="s">
@@ -3870,20 +3563,20 @@
         <v>132</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="98">
       <c r="A98" t="s">
         <v>105</v>
       </c>
-      <c r="B98">
-        <v>2013</v>
-      </c>
-      <c r="C98" s="3">
+      <c r="B98" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C98" t="n">
         <v>1938870.4882347418</v>
       </c>
-      <c r="D98">
+      <c r="D98" t="n">
         <v>353727.97973737156</v>
       </c>
-      <c r="E98">
+      <c r="E98" t="n">
         <v>0.18244023099213072</v>
       </c>
       <c r="F98" t="s">
@@ -3902,53 +3595,53 @@
         <v>132</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A99" s="1" t="s">
+    <row r="99">
+      <c r="A99" t="s">
         <v>106</v>
       </c>
-      <c r="B99" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C99" s="2">
+      <c r="B99" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C99" t="n">
         <v>2250572.0318013267</v>
       </c>
-      <c r="D99" s="1">
-        <v>354021.63476924971</v>
-      </c>
-      <c r="E99" s="1">
+      <c r="D99" t="n">
+        <v>354021.6347692497</v>
+      </c>
+      <c r="E99" t="n">
         <v>0.15730295665582217</v>
       </c>
-      <c r="F99" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G99" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H99" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I99" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="J99" s="1" t="s">
+      <c r="F99" t="s">
+        <v>121</v>
+      </c>
+      <c r="G99" t="s">
+        <v>122</v>
+      </c>
+      <c r="H99" t="s">
+        <v>123</v>
+      </c>
+      <c r="I99" t="s">
+        <v>124</v>
+      </c>
+      <c r="J99" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="100" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="100">
       <c r="A100" t="s">
         <v>107</v>
       </c>
-      <c r="B100">
-        <v>1984</v>
-      </c>
-      <c r="C100" s="3">
+      <c r="B100" t="n">
+        <v>1984.0</v>
+      </c>
+      <c r="C100" t="n">
         <v>220910.51048170237</v>
       </c>
-      <c r="D100">
+      <c r="D100" t="n">
         <v>56130.539466759525</v>
       </c>
-      <c r="E100">
-        <v>0.25408722900673719</v>
+      <c r="E100" t="n">
+        <v>0.2540872290067372</v>
       </c>
       <c r="F100" t="s">
         <v>121</v>
@@ -3966,20 +3659,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="101">
       <c r="A101" t="s">
         <v>108</v>
       </c>
-      <c r="B101">
-        <v>1987</v>
-      </c>
-      <c r="C101" s="3">
+      <c r="B101" t="n">
+        <v>1987.0</v>
+      </c>
+      <c r="C101" t="n">
         <v>241438.2484739793</v>
       </c>
-      <c r="D101">
-        <v>54847.878837638738</v>
-      </c>
-      <c r="E101">
+      <c r="D101" t="n">
+        <v>54847.87883763874</v>
+      </c>
+      <c r="E101" t="n">
         <v>0.22717145764727456</v>
       </c>
       <c r="F101" t="s">
@@ -3998,20 +3691,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="102">
       <c r="A102" t="s">
         <v>109</v>
       </c>
-      <c r="B102">
-        <v>1990</v>
-      </c>
-      <c r="C102" s="3">
+      <c r="B102" t="n">
+        <v>1990.0</v>
+      </c>
+      <c r="C102" t="n">
         <v>157295.10810108116</v>
       </c>
-      <c r="D102">
-        <v>47129.364084270906</v>
-      </c>
-      <c r="E102">
+      <c r="D102" t="n">
+        <v>47129.36408427091</v>
+      </c>
+      <c r="E102" t="n">
         <v>0.29962383861286124</v>
       </c>
       <c r="F102" t="s">
@@ -4030,20 +3723,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="103">
       <c r="A103" t="s">
         <v>110</v>
       </c>
-      <c r="B103">
-        <v>1993</v>
-      </c>
-      <c r="C103" s="3">
-        <v>483482.05804852961</v>
-      </c>
-      <c r="D103">
+      <c r="B103" t="n">
+        <v>1993.0</v>
+      </c>
+      <c r="C103" t="n">
+        <v>483482.0580485296</v>
+      </c>
+      <c r="D103" t="n">
         <v>108639.97592897959</v>
       </c>
-      <c r="E103">
+      <c r="E103" t="n">
         <v>0.22470322139249857</v>
       </c>
       <c r="F103" t="s">
@@ -4062,20 +3755,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104">
       <c r="A104" t="s">
         <v>111</v>
       </c>
-      <c r="B104">
-        <v>1996</v>
-      </c>
-      <c r="C104" s="3">
+      <c r="B104" t="n">
+        <v>1996.0</v>
+      </c>
+      <c r="C104" t="n">
         <v>771412.7700741177</v>
       </c>
-      <c r="D104">
-        <v>203553.81128867989</v>
-      </c>
-      <c r="E104">
+      <c r="D104" t="n">
+        <v>203553.8112886799</v>
+      </c>
+      <c r="E104" t="n">
         <v>0.26387145661216155</v>
       </c>
       <c r="F104" t="s">
@@ -4094,21 +3787,21 @@
         <v>125</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105">
       <c r="A105" t="s">
         <v>112</v>
       </c>
-      <c r="B105">
-        <v>1999</v>
-      </c>
-      <c r="C105" s="3">
-        <v>727063.47154458845</v>
-      </c>
-      <c r="D105">
-        <v>388566.00749154738</v>
-      </c>
-      <c r="E105">
-        <v>0.53443203062597799</v>
+      <c r="B105" t="n">
+        <v>1999.0</v>
+      </c>
+      <c r="C105" t="n">
+        <v>727063.4715445885</v>
+      </c>
+      <c r="D105" t="n">
+        <v>388566.0074915474</v>
+      </c>
+      <c r="E105" t="n">
+        <v>0.534432030625978</v>
       </c>
       <c r="F105" t="s">
         <v>121</v>
@@ -4126,21 +3819,21 @@
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="106">
       <c r="A106" t="s">
         <v>113</v>
       </c>
-      <c r="B106">
-        <v>2001</v>
-      </c>
-      <c r="C106" s="3">
-        <v>673155.06149275915</v>
-      </c>
-      <c r="D106">
+      <c r="B106" t="n">
+        <v>2001.0</v>
+      </c>
+      <c r="C106" t="n">
+        <v>673155.0614927592</v>
+      </c>
+      <c r="D106" t="n">
         <v>222003.02456328887</v>
       </c>
-      <c r="E106">
-        <v>0.32979477874085161</v>
+      <c r="E106" t="n">
+        <v>0.3297947787408516</v>
       </c>
       <c r="F106" t="s">
         <v>121</v>
@@ -4158,20 +3851,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="107">
       <c r="A107" t="s">
         <v>114</v>
       </c>
-      <c r="B107">
-        <v>2003</v>
-      </c>
-      <c r="C107" s="3">
+      <c r="B107" t="n">
+        <v>2003.0</v>
+      </c>
+      <c r="C107" t="n">
         <v>457421.5614838581</v>
       </c>
-      <c r="D107">
-        <v>72014.762353295751</v>
-      </c>
-      <c r="E107">
+      <c r="D107" t="n">
+        <v>72014.76235329575</v>
+      </c>
+      <c r="E107" t="n">
         <v>0.157436309122995</v>
       </c>
       <c r="F107" t="s">
@@ -4190,20 +3883,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="108" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="108">
       <c r="A108" t="s">
         <v>115</v>
       </c>
-      <c r="B108">
-        <v>2005</v>
-      </c>
-      <c r="C108" s="3">
-        <v>764901.40612710686</v>
-      </c>
-      <c r="D108">
+      <c r="B108" t="n">
+        <v>2005.0</v>
+      </c>
+      <c r="C108" t="n">
+        <v>764901.4061271069</v>
+      </c>
+      <c r="D108" t="n">
         <v>146628.12305767962</v>
       </c>
-      <c r="E108">
+      <c r="E108" t="n">
         <v>0.19169545497385818</v>
       </c>
       <c r="F108" t="s">
@@ -4222,20 +3915,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="109">
       <c r="A109" t="s">
         <v>116</v>
       </c>
-      <c r="B109">
-        <v>2007</v>
-      </c>
-      <c r="C109" s="3">
-        <v>688179.75351276679</v>
-      </c>
-      <c r="D109">
+      <c r="B109" t="n">
+        <v>2007.0</v>
+      </c>
+      <c r="C109" t="n">
+        <v>688179.7535127668</v>
+      </c>
+      <c r="D109" t="n">
         <v>114172.16510181692</v>
       </c>
-      <c r="E109">
+      <c r="E109" t="n">
         <v>0.16590456856516464</v>
       </c>
       <c r="F109" t="s">
@@ -4254,20 +3947,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="110" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="110">
       <c r="A110" t="s">
         <v>117</v>
       </c>
-      <c r="B110">
-        <v>2009</v>
-      </c>
-      <c r="C110" s="3">
-        <v>649449.18614240282</v>
-      </c>
-      <c r="D110">
+      <c r="B110" t="n">
+        <v>2009.0</v>
+      </c>
+      <c r="C110" t="n">
+        <v>649449.1861424028</v>
+      </c>
+      <c r="D110" t="n">
         <v>117760.62859978729</v>
       </c>
-      <c r="E110">
+      <c r="E110" t="n">
         <v>0.18132385275476542</v>
       </c>
       <c r="F110" t="s">
@@ -4286,20 +3979,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="111" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="111">
       <c r="A111" t="s">
         <v>118</v>
       </c>
-      <c r="B111">
-        <v>2011</v>
-      </c>
-      <c r="C111" s="3">
-        <v>778669.25205430645</v>
-      </c>
-      <c r="D111">
+      <c r="B111" t="n">
+        <v>2011.0</v>
+      </c>
+      <c r="C111" t="n">
+        <v>778669.2520543064</v>
+      </c>
+      <c r="D111" t="n">
         <v>135505.97201564326</v>
       </c>
-      <c r="E111">
+      <c r="E111" t="n">
         <v>0.17402250269693803</v>
       </c>
       <c r="F111" t="s">
@@ -4318,20 +4011,20 @@
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="112">
       <c r="A112" t="s">
         <v>119</v>
       </c>
-      <c r="B112">
-        <v>2013</v>
-      </c>
-      <c r="C112" s="3">
+      <c r="B112" t="n">
+        <v>2013.0</v>
+      </c>
+      <c r="C112" t="n">
         <v>1298443.4559864458</v>
       </c>
-      <c r="D112">
+      <c r="D112" t="n">
         <v>213516.032964235</v>
       </c>
-      <c r="E112">
+      <c r="E112" t="n">
         <v>0.16443999311623766</v>
       </c>
       <c r="F112" t="s">
@@ -4350,39 +4043,39 @@
         <v>125</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A113" s="1" t="s">
+    <row r="113">
+      <c r="A113" t="s">
         <v>120</v>
       </c>
-      <c r="B113" s="1">
-        <v>2015</v>
-      </c>
-      <c r="C113" s="2">
+      <c r="B113" t="n">
+        <v>2015.0</v>
+      </c>
+      <c r="C113" t="n">
         <v>1140406.7073026828</v>
       </c>
-      <c r="D113" s="1">
-        <v>176812.03238420581</v>
-      </c>
-      <c r="E113" s="1">
+      <c r="D113" t="n">
+        <v>176812.0323842058</v>
+      </c>
+      <c r="E113" t="n">
         <v>0.15504296077178104</v>
       </c>
-      <c r="F113" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="G113" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="H113" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="I113" s="1" t="s">
+      <c r="F113" t="s">
+        <v>121</v>
+      </c>
+      <c r="G113" t="s">
+        <v>122</v>
+      </c>
+      <c r="H113" t="s">
+        <v>123</v>
+      </c>
+      <c r="I113" t="s">
         <v>125</v>
       </c>
-      <c r="J113" s="1" t="s">
+      <c r="J113" t="s">
         <v>125</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>